<commit_message>
With changes made to TCH_IND (pre changes made by Bryce)
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/CO2SConstraint.xlsx
+++ b/SATIM/DataSpreadsheets/CO2SConstraint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47909EEA-6E26-4D2C-9E59-AB9D64442785}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6701B3C-7F78-4449-A011-196CF72065B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="0" windowWidth="28770" windowHeight="15570" xr2:uid="{DD1845FD-3FD2-4947-96E6-D580C1150EEB}"/>
   </bookViews>
@@ -1597,7 +1597,7 @@
   <dimension ref="B1:AG4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
+      <selection activeCell="U3" sqref="U3:AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>